<commit_message>
Updated lookup tutorial materials
</commit_message>
<xml_diff>
--- a/excel-lookup-function-tutorial.xlsx
+++ b/excel-lookup-function-tutorial.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8760"/>
+    <workbookView xWindow="288" yWindow="420" windowWidth="18852" windowHeight="6636"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Functions Tutorial" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,13 @@
   <definedNames>
     <definedName name="data">'Lookup Functions Tutorial'!$A$3:$C$12</definedName>
     <definedName name="data_header">'Lookup Functions Tutorial'!$A$3:$C$3</definedName>
-    <definedName name="FtoC_conv">'Lookup Functions Tutorial'!$E$27</definedName>
-    <definedName name="SecCode1">'Lookup Functions Tutorial'!$H$93:$K$100</definedName>
-    <definedName name="SecCode1_Color">'Lookup Functions Tutorial'!$H$93:$H$100</definedName>
-    <definedName name="SecCode1_h">'Lookup Functions Tutorial'!$H$93:$K$93</definedName>
-    <definedName name="SecCode2">'Lookup Functions Tutorial'!$M$93:$P$100</definedName>
-    <definedName name="SecCode2_Color">'Lookup Functions Tutorial'!$M$93:$M$100</definedName>
-    <definedName name="SecCode2_h">'Lookup Functions Tutorial'!$M$93:$P$93</definedName>
+    <definedName name="FtoC_conv">'Lookup Functions Tutorial'!$E$26</definedName>
+    <definedName name="SecCode1">'Lookup Functions Tutorial'!$F$100:$I$107</definedName>
+    <definedName name="SecCode1_Color">'Lookup Functions Tutorial'!$F$100:$F$107</definedName>
+    <definedName name="SecCode1_h">'Lookup Functions Tutorial'!$F$100:$I$100</definedName>
+    <definedName name="SecCode2">'Lookup Functions Tutorial'!$K$100:$N$107</definedName>
+    <definedName name="SecCode2_Color">'Lookup Functions Tutorial'!$K$100:$K$107</definedName>
+    <definedName name="SecCode2_h">'Lookup Functions Tutorial'!$K$100:$N$100</definedName>
     <definedName name="Spare">'[1]Control Room'!#REF!</definedName>
     <definedName name="TestData">'Lookup Functions Tutorial'!$A$3:$C$12</definedName>
     <definedName name="TestData_header">'Lookup Functions Tutorial'!$A$3:$C$3</definedName>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="127">
   <si>
     <t>Excel Lookup-Functions Tutorial</t>
   </si>
@@ -101,13 +101,7 @@
     <t>Example using INDEX, but with a "range name"</t>
   </si>
   <si>
-    <t>in its coordinates, potentially several times if you continue to use the information there several times. Second, from looking at the formula, it's impossible to know what the contents of the table are.</t>
-  </si>
-  <si>
-    <t>Giving a group of cells a "range name" makes referring to tables easier, and makes formulas more transparent and readable.</t>
-  </si>
-  <si>
-    <t>If you highlight a cell (or a range of cells), click in there and type in another word, then you've just created that alias. As another quick example, I've done this with cell C25, and used it in C27 and C28:</t>
+    <t>it's referencing. Giving a group of cells a "range name" makes referring to tables easier, and makes formulas more transparent and readable.</t>
   </si>
   <si>
     <t>Temp F</t>
@@ -147,7 +141,7 @@
     <t>Concatenating Text</t>
   </si>
   <si>
-    <t>You concatenate text using the "&amp;" operator. Take a look at the example below:</t>
+    <t>Just like the plus sign (+) is a "binary" operator which adds two things together, an ampersand (&amp;) is a binary operator which glues two text strings together:</t>
   </si>
   <si>
     <t>Note that text has to be surrounded by double-quotes. Otherwise Excel will try to look for a range name of that name or for a key word, or will just plain get confused. Contrast the above formula with this one:</t>
@@ -156,10 +150,43 @@
     <t>Using Dollar Signs to Make Cell References Smarter</t>
   </si>
   <si>
-    <t>One thing</t>
-  </si>
-  <si>
-    <t>The other</t>
+    <t xml:space="preserve">Excel tries to be helpful whenever it can. If a cell's formula references a neighbor, and you copy and paste that formula to another cell, Excel updates both the row and the column of </t>
+  </si>
+  <si>
+    <t>the reference so that the new formula has the same relative positioning.</t>
+  </si>
+  <si>
+    <t>Consider the following example where we cleverly design a formula to cue off of its context in the table. This is smart--we design one formula, and (ideally) it works perfectly, using</t>
+  </si>
+  <si>
+    <t>an analog same logic we use in reading the table: calculation should be based off of the radius value on the same row, and have the calculation type of the column it's under.</t>
+  </si>
+  <si>
+    <t>However, when we copy the formula down, the updating references keep us from getting what we want. Select the various cells in the second table, and hit "F2" to visually display the referneces.</t>
+  </si>
+  <si>
+    <t>To fix this problem, use "$"s, strategically placed to the left of cell references that we want to keep from updating.</t>
+  </si>
+  <si>
+    <t>(Note that range names always represent absolute references, as we might expect.)</t>
+  </si>
+  <si>
+    <t>Drafting our clever formula…</t>
+  </si>
+  <si>
+    <t>Naively copying our formula to other cells…</t>
+  </si>
+  <si>
+    <t>Smartly using "$"s to fix row and column elements the way we want</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Circumference</t>
   </si>
   <si>
     <t>Highly Efficient Index() Functions - Using it all together</t>
@@ -168,7 +195,7 @@
     <t>Using range names, you can just reference the data tables and lists that you want very clearly and simply.</t>
   </si>
   <si>
-    <t>in the table above.</t>
+    <t>it knows how to look there.</t>
   </si>
   <si>
     <t>Inside the first MATCH function, I use concatenation to build a unique row idea to look up in the above table.</t>
@@ -183,10 +210,10 @@
     <t>Storing and hiding stuff under the hood - Group and Ungroup vs. Hide and Unhide</t>
   </si>
   <si>
-    <t>In the table above, the names on the left and test names on the top are both the names of the variables in the data (at the very top) and labels that we're happy to apply. In general, the labels you want will</t>
-  </si>
-  <si>
-    <t>Ay! You found me!!</t>
+    <t>In the table above, the names on the left and test names on the top are both the names of the variables in the data (at the very top) and labels that we're happy to apply. In general, the labels you want can</t>
+  </si>
+  <si>
+    <t>Ye found me pot of gold!</t>
   </si>
   <si>
     <t>differ from your variable names and column titles. The solution is to store your variables names in one column (for reference) and label names in another column (for display). You can obtain this solution</t>
@@ -234,13 +261,13 @@
     <t>Third Test</t>
   </si>
   <si>
-    <t>Mr. Zanoni</t>
-  </si>
-  <si>
-    <t>Mr. Goerge</t>
-  </si>
-  <si>
-    <t>Mr. Mader</t>
+    <t>Wlad W.</t>
+  </si>
+  <si>
+    <t>Bob G.</t>
+  </si>
+  <si>
+    <t>Nick M.</t>
   </si>
   <si>
     <r>
@@ -415,13 +442,19 @@
     </r>
   </si>
   <si>
+    <t>Red</t>
+  </si>
+  <si>
     <t>Secret Code #1</t>
   </si>
   <si>
     <t>Secret Code #2</t>
   </si>
   <si>
-    <t>Red</t>
+    <t>Code #1</t>
+  </si>
+  <si>
+    <t>Code #2</t>
   </si>
   <si>
     <t>Color</t>
@@ -436,10 +469,10 @@
     <t>Illinois</t>
   </si>
   <si>
-    <t>Code #1</t>
-  </si>
-  <si>
-    <t>Code #2</t>
+    <t>SecCode1</t>
+  </si>
+  <si>
+    <t>SecCode2</t>
   </si>
   <si>
     <t>ž</t>
@@ -458,12 +491,6 @@
   </si>
   <si>
     <t>ä</t>
-  </si>
-  <si>
-    <t>SecCode1</t>
-  </si>
-  <si>
-    <t>SecCode2</t>
   </si>
   <si>
     <t>Orange</t>
@@ -596,7 +623,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -674,8 +701,30 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
-      <color indexed="17"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -697,13 +746,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="13">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -730,13 +774,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -881,7 +955,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -903,6 +977,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -912,7 +987,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -969,6 +1044,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="12" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -984,7 +1062,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -992,19 +1087,16 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1012,10 +1104,16 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1025,7 +1123,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1034,38 +1132,26 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1075,16 +1161,16 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="30">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="2"/>
     <cellStyle name="Normal 11" xfId="3"/>
@@ -1106,14 +1192,15 @@
     <cellStyle name="Normal 26" xfId="19"/>
     <cellStyle name="Normal 27" xfId="1"/>
     <cellStyle name="Normal 28" xfId="20"/>
-    <cellStyle name="Normal 3" xfId="21"/>
-    <cellStyle name="Normal 4" xfId="22"/>
-    <cellStyle name="Normal 4 2" xfId="23"/>
-    <cellStyle name="Normal 5" xfId="24"/>
-    <cellStyle name="Normal 6" xfId="25"/>
-    <cellStyle name="Normal 7" xfId="26"/>
-    <cellStyle name="Normal 8" xfId="27"/>
-    <cellStyle name="Normal 9" xfId="28"/>
+    <cellStyle name="Normal 29" xfId="21"/>
+    <cellStyle name="Normal 3" xfId="22"/>
+    <cellStyle name="Normal 4" xfId="23"/>
+    <cellStyle name="Normal 4 2" xfId="24"/>
+    <cellStyle name="Normal 5" xfId="25"/>
+    <cellStyle name="Normal 6" xfId="26"/>
+    <cellStyle name="Normal 7" xfId="27"/>
+    <cellStyle name="Normal 8" xfId="28"/>
+    <cellStyle name="Normal 9" xfId="29"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1131,10 +1218,16 @@
     <sheetNames>
       <sheetName val="Lookup Functions Tutorial"/>
       <sheetName val="Control Room"/>
+      <sheetName val="Table X - Regression Estimates"/>
+      <sheetName val="table1"/>
+      <sheetName val="desc_stats"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1427,30 +1520,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:P120"/>
+  <dimension ref="A1:P135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="80"/>
-    <col min="2" max="2" width="10.85546875" style="80" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="80"/>
-    <col min="4" max="4" width="12.7109375" style="80" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="80"/>
+    <col min="1" max="1" width="9.109375" style="89" customWidth="1"/>
+    <col min="2" max="3" width="10" style="89" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="89" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" style="89" customWidth="1"/>
+    <col min="6" max="7" width="9.109375" style="89" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" style="89" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" style="89" customWidth="1"/>
+    <col min="10" max="11" width="9.109375" style="89" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" style="89" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="9.109375" style="89" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="89" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1458,7 +1557,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1472,7 +1571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1490,7 +1589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1517,7 +1616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -1544,7 +1643,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1572,7 +1671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1600,7 +1699,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
@@ -1616,7 +1715,7 @@
         <v>Wladimir_Test3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -1632,7 +1731,7 @@
         <v>Bob_Test1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1648,7 +1747,7 @@
         <v>Bob_Test2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1664,865 +1763,982 @@
         <v>Bob_Test3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:11" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
         <f>INDEX(A3:C12, 5, 3)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
     </row>
-    <row r="18" spans="1:8" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="26" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="str">
-        <f>"In the example above, the first argument of the table is 'A"&amp;ROW(A3)&amp;":C"&amp;ROW(A12)&amp;"'. That makes sense, but has a few limitations. If you want to reference it from other sheets, you need to go to the source table and enter"</f>
-        <v>In the example above, the first argument of the table is 'A3:C12'. That makes sense, but has a few limitations. If you want to reference it from other sheets, you need to go to the source table and enter</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+        <f>"In the example above, the first argument of the table is 'A"&amp;ROW(A3)&amp;":C"&amp;ROW(A12)&amp;"'. While that's a familiar reference, it's got a limitation: it's hard for people to know semantically what"</f>
+        <v>In the example above, the first argument of the table is 'A3:C12'. While that's a familiar reference, it's got a limitation: it's hard for people to know semantically what</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="28">
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="29">
         <f>INDEX(TestData, 5, 3)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27"/>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+    </row>
+    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="str">
+        <f>"A range name is just an alias for a cell. This cell is named 'A"&amp;ROW(A23)&amp;"', and if you have it selected, then you'll see a box reading 'A"&amp;ROW(A23)&amp;"' at the top left of your screen, below the File menu, just past the toolbars."</f>
+        <v>A range name is just an alias for a cell. This cell is named 'A23', and if you have it selected, then you'll see a box reading 'A23' at the top left of your screen, below the File menu, just past the toolbars.</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="str">
-        <f>"A range name is just an alias for a cell. This cell is named 'A"&amp;ROW(A24)&amp;"', and if you have it selected, then you'll see a box reading 'A"&amp;ROW(A24)&amp;"' at the top left of your screen, below the File menu, just past the toolbars."</f>
-        <v>A range name is just an alias for a cell. This cell is named 'A24', and if you have it selected, then you'll see a box reading 'A24' at the top left of your screen, below the File menu, just past the toolbars.</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+        <f>"If you highlight a cell (or a range of cells), click in there and type in another word, then you've just created that alias. As another quick example, I've done this with cell E"&amp;ROW(FtoC_conv)&amp;", and used it in C"&amp;ROW(C27)&amp;" and C"&amp;ROW(C28)&amp;":"</f>
+        <v>If you highlight a cell (or a range of cells), click in there and type in another word, then you've just created that alias. As another quick example, I've done this with cell E26, and used it in C27 and C28:</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="29">
+      <c r="E26" s="30">
         <f>5/9</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F26" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="32"/>
+      <c r="H26" s="33"/>
+    </row>
+    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>85</v>
+      </c>
+      <c r="C27" s="34">
+        <f>FtoC_conv*(B27-32)</f>
+        <v>29.444444444444446</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>40</v>
+      </c>
+      <c r="C28" s="34">
+        <f>FtoC_conv*(B28-32)</f>
+        <v>4.4444444444444446</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:8" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="31"/>
-      <c r="H27" s="32"/>
-    </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="8">
-        <v>85</v>
-      </c>
-      <c r="C28" s="33">
-        <f>FtoC_conv*(B28-32)</f>
-        <v>29.444444444444446</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="8">
-        <v>40</v>
-      </c>
-      <c r="C29" s="33">
-        <f>FtoC_conv*(B29-32)</f>
-        <v>4.4444444444444446</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:1" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="24">
+    </row>
+    <row r="33" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24">
         <f>MATCH("Bob_Test3", TestData_ID, 0)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:1" s="26" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
+    <row r="38" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:1" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="36" t="str">
+    <row r="39" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="str">
         <f>"Math"&amp;"Rulez"</f>
         <v>MathRulez</v>
       </c>
     </row>
-    <row r="41" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="36" t="e">
+    <row r="40" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="e">
         <f>Math&amp;Rulez</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="43" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:1" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
+    <row r="42" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:1" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="23" t="str">
-        <f>"If you reference a cell in a formula and then drag or copy that formula, Excel will move the reference over as well. For example, take a look at cell B"&amp;ROW($B$49)&amp;". I created that cell reference, and just copied it down."</f>
-        <v>If you reference a cell in a formula and then drag or copy that formula, Excel will move the reference over as well. For example, take a look at cell B49. I created that cell reference, and just copied it down.</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="22" t="str">
-        <f>"If, however, you don't want the reference to update, you can put a dollar sign in the name of the cell to freeze either the column, the row, or both. Below, I typed in cell A"&amp;ROW($A$49)&amp;", referenced it in cell B"&amp;ROW($B$49)&amp;", but froze the"</f>
-        <v>If, however, you don't want the reference to update, you can put a dollar sign in the name of the cell to freeze either the column, the row, or both. Below, I typed in cell A49, referenced it in cell B49, but froze the</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="str">
-        <f>"fact that the reference is to column "&amp;CHAR(34)&amp;"A"&amp;CHAR(34)&amp;". When I copied that formula to the right, it still references column A. However, when I copy it down to B"&amp;ROW($C$50)&amp;", it updates to "&amp;CHAR(34)&amp;"=$A"&amp;ROW($B$50)&amp;CHAR(34)&amp;" because the row isn't frozen."</f>
-        <v>fact that the reference is to column "A". When I copied that formula to the right, it still references column A. However, when I copy it down to B50, it updates to "=$A50" because the row isn't frozen.</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="22" t="s">
+    <row r="46" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="37" t="str">
-        <f t="shared" ref="B49:D50" si="2">$A49</f>
-        <v>One thing</v>
-      </c>
-      <c r="C49" s="37" t="str">
+    </row>
+    <row r="47" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A51" s="39"/>
+    </row>
+    <row r="52" spans="1:12" s="41" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A52" s="40"/>
+      <c r="B52" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="J52" s="41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A53" s="39"/>
+      <c r="B53" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="J53" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="K53" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="L53" s="43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A54" s="39"/>
+      <c r="B54" s="44">
+        <v>1</v>
+      </c>
+      <c r="C54" s="45">
+        <f>PI()*IF(C53="Area", B54^2, B54*2)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="D54" s="45"/>
+      <c r="F54" s="44">
+        <v>1</v>
+      </c>
+      <c r="G54" s="45">
+        <f>PI()*IF(G53="Area", F54^2, F54*2)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="H54" s="45">
+        <f t="shared" ref="H54:H56" si="2">PI()*IF(H53="Area", G54^2, G54*2)</f>
+        <v>19.739208802178716</v>
+      </c>
+      <c r="J54" s="44">
+        <v>1</v>
+      </c>
+      <c r="K54" s="45">
+        <f>PI()*IF(K$53="Area", $J54^2, $J54*2)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="L54" s="45">
+        <f t="shared" ref="L54:L56" si="3">PI()*IF(L$53="Area", $J54^2, $J54*2)</f>
+        <v>6.2831853071795862</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A55" s="39"/>
+      <c r="B55" s="44">
+        <v>2</v>
+      </c>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="F55" s="44">
+        <v>2</v>
+      </c>
+      <c r="G55" s="45">
+        <f t="shared" ref="G55:G56" si="4">PI()*IF(G54="Area", F55^2, F55*2)</f>
+        <v>12.566370614359172</v>
+      </c>
+      <c r="H55" s="45">
         <f t="shared" si="2"/>
-        <v>One thing</v>
-      </c>
-      <c r="D49" s="37" t="str">
+        <v>78.956835208714864</v>
+      </c>
+      <c r="J55" s="44">
+        <v>2</v>
+      </c>
+      <c r="K55" s="45">
+        <f t="shared" ref="K55:L56" si="5">PI()*IF(K$53="Area", $J55^2, $J55*2)</f>
+        <v>12.566370614359172</v>
+      </c>
+      <c r="L55" s="45">
+        <f t="shared" si="3"/>
+        <v>12.566370614359172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A56" s="39"/>
+      <c r="B56" s="44">
+        <v>3</v>
+      </c>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="F56" s="44">
+        <v>3</v>
+      </c>
+      <c r="G56" s="45">
+        <f t="shared" si="4"/>
+        <v>18.849555921538759</v>
+      </c>
+      <c r="H56" s="45">
         <f t="shared" si="2"/>
-        <v>One thing</v>
-      </c>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-    </row>
-    <row r="50" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v>The other</v>
-      </c>
-      <c r="C50" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v>The other</v>
-      </c>
-      <c r="D50" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v>The other</v>
-      </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-    </row>
-    <row r="51" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:6" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+        <v>118.4352528130723</v>
+      </c>
+      <c r="J56" s="44">
+        <v>3</v>
+      </c>
+      <c r="K56" s="45">
+        <f t="shared" si="5"/>
+        <v>28.274333882308138</v>
+      </c>
+      <c r="L56" s="45">
+        <f t="shared" si="3"/>
+        <v>18.849555921538759</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A57" s="39"/>
+    </row>
+    <row r="58" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:12" s="26" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A59" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+    <row r="61" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="38">
-        <f t="shared" ref="B54:D56" si="3">INDEX(TestData, MATCH($A54&amp;"_"&amp;B$53, TestData_ID, 0), MATCH("Score", TestData_header, 0))</f>
+      <c r="B61" s="46">
+        <f t="shared" ref="B61:D63" si="6">INDEX(TestData, MATCH($A61&amp;"_"&amp;B$60, TestData_ID, 0), MATCH("Score", TestData_header, 0))</f>
         <v>50</v>
       </c>
-      <c r="C54" s="38">
-        <f t="shared" si="3"/>
+      <c r="C61" s="46">
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
-      <c r="D54" s="38">
-        <f t="shared" si="3"/>
+      <c r="D61" s="46">
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+    <row r="62" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="38">
-        <f t="shared" si="3"/>
+      <c r="B62" s="46">
+        <f t="shared" si="6"/>
         <v>95</v>
       </c>
-      <c r="C55" s="38">
-        <f t="shared" si="3"/>
+      <c r="C62" s="46">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="D55" s="38">
-        <f t="shared" si="3"/>
+      <c r="D62" s="46">
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
+    <row r="63" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="38">
-        <f t="shared" si="3"/>
+      <c r="B63" s="46">
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="C56" s="38">
-        <f t="shared" si="3"/>
+      <c r="C63" s="46">
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
-      <c r="D56" s="38">
-        <f t="shared" si="3"/>
+      <c r="D63" s="46">
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="40" t="str">
-        <f>"By using the MATCH function, this formula becomes smart enough to use it's own context to know what to look for. I.e., cell C"&amp;ROW($C$56)&amp;" knows that it's in "&amp;CHAR(34)&amp;"Nick"&amp;CHAR(34)&amp;"'s row and the "&amp;CHAR(34)&amp;"Test2"&amp;CHAR(34)&amp;" column, so that's where it looks"</f>
-        <v>By using the MATCH function, this formula becomes smart enough to use it's own context to know what to look for. I.e., cell C56 knows that it's in "Nick"'s row and the "Test2" column, so that's where it looks</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="41" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="42" t="s">
+    <row r="64" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="48" t="str">
+        <f>"By using the MATCH function, this formula becomes smart enough to use it's own context to know what to look for. I.e., cell C"&amp;ROW($C$63)&amp;" knows that it's in the row for "&amp;CHAR(34)&amp;"Nick"&amp;CHAR(34)&amp;" and the column for "&amp;CHAR(34)&amp;"Test2"&amp;CHAR(34)&amp;", and"</f>
+        <v>By using the MATCH function, this formula becomes smart enough to use it's own context to know what to look for. I.e., cell C63 knows that it's in the row for "Nick" and the column for "Test2", and</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="52" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="54" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A71" s="53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="57" customFormat="1" ht="29.4" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D73" s="58"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="60"/>
+      <c r="G73" s="61"/>
+      <c r="H73" s="62"/>
+      <c r="I73" s="63"/>
+    </row>
+    <row r="74" spans="1:9" s="54" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="55" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="55"/>
+    </row>
+    <row r="77" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="64"/>
+      <c r="C78" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="64"/>
+      <c r="B79" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="D79" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="E79" s="67" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" s="69">
+        <f t="shared" ref="C80:E82" si="7">INDEX(TestData, MATCH($A80&amp;"_"&amp;C$78, TestData_ID, 0),MATCH("Score", TestData_header, 0))</f>
+        <v>50</v>
+      </c>
+      <c r="D80" s="69">
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="43" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="45" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="44" t="s">
+      <c r="E80" s="69">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="C81" s="69">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="D81" s="69">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="E81" s="69">
+        <f t="shared" si="7"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" s="69">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="D82" s="69">
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="50" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="47" customFormat="1" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="48" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="48" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="48"/>
-    </row>
-    <row r="70" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="51" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="51"/>
-      <c r="C71" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="51"/>
-      <c r="B72" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="C72" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="D72" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="E72" s="54" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="C73" s="56">
-        <f t="shared" ref="C73:E75" si="4">INDEX(TestData, MATCH($A73&amp;"_"&amp;C$71, TestData_ID, 0),MATCH("Score", TestData_header, 0))</f>
-        <v>50</v>
-      </c>
-      <c r="D73" s="56">
-        <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="E73" s="56">
-        <f t="shared" si="4"/>
+      <c r="E82" s="69">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="64"/>
+    </row>
+    <row r="84" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="64" t="str">
+        <f>"forget what's there. For example, you would probably never have realized that row "&amp;ROW(A70)&amp;" is hidden! You'd only notice if you already knew it was hidden, or were paying very close attention to the row numbers, in which case "</f>
+        <v xml:space="preserve">forget what's there. For example, you would probably never have realized that row 70 is hidden! You'd only notice if you already knew it was hidden, or were paying very close attention to the row numbers, in which case </v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="64"/>
+    </row>
+    <row r="88" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="64" t="str">
+        <f>"As you can clearly see, we've got a plus sign on row "&amp;ROW($A$73)&amp;"! Open it up! And, for a nice example of how it can be used, see the example on INDIRECT() below!"</f>
+        <v>As you can clearly see, we've got a plus sign on row 73! Open it up! And, for a nice example of how it can be used, see the example on INDIRECT() below!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="70"/>
+    </row>
+    <row r="92" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A92" s="71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="48"/>
+    </row>
+    <row r="99" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="48"/>
+      <c r="B99" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C99" s="73"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="74" t="s">
+        <v>70</v>
+      </c>
+      <c r="G99" s="75"/>
+      <c r="H99" s="74"/>
+      <c r="I99" s="75"/>
+      <c r="J99" s="76"/>
+      <c r="K99" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="L99" s="75"/>
+      <c r="M99" s="74"/>
+      <c r="N99" s="75"/>
+    </row>
+    <row r="100" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="20"/>
+      <c r="B100" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="C100" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="D100" s="8"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="G100" s="77" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B74" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="C74" s="56">
-        <f t="shared" si="4"/>
-        <v>95</v>
-      </c>
-      <c r="D74" s="56">
-        <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="E74" s="56">
-        <f t="shared" si="4"/>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="C75" s="56">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="D75" s="56">
-        <f t="shared" si="4"/>
-        <v>37</v>
-      </c>
-      <c r="E75" s="56">
-        <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="51"/>
-    </row>
-    <row r="77" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="51" t="str">
-        <f>"forget what's there. For example, you would probably never have realized that row "&amp;ROW(A63)&amp;" is hidden! You'd only notice if you already knew it was hidden, or were paying very close attention to the row numbers, in which case "</f>
-        <v xml:space="preserve">forget what's there. For example, you would probably never have realized that row 63 is hidden! You'd only notice if you already knew it was hidden, or were paying very close attention to the row numbers, in which case </v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="51"/>
-    </row>
-    <row r="81" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="51" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="51" t="str">
-        <f>"As you can clearly see, we've got a plus sign on row "&amp;ROW($A$66)&amp;"! Open it up! And, for a nice example of how it can be used, see the example on INDIRECT() below!"</f>
-        <v>As you can clearly see, we've got a plus sign on row 66! Open it up! And, for a nice example of how it can be used, see the example on INDIRECT() below!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="57"/>
-    </row>
-    <row r="85" spans="1:16" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="58" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="40"/>
-    </row>
-    <row r="92" spans="1:16" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="59"/>
-      <c r="C92" s="61"/>
-      <c r="D92" s="62"/>
-      <c r="E92" s="61"/>
-      <c r="F92" s="63"/>
-      <c r="G92" s="63"/>
-      <c r="H92" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="I92" s="65"/>
-      <c r="J92" s="64"/>
-      <c r="K92" s="65"/>
-      <c r="M92" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="N92" s="65"/>
-      <c r="O92" s="64"/>
-      <c r="P92" s="65"/>
-    </row>
-    <row r="93" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="40"/>
-      <c r="B93" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="C93" s="67"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="27"/>
-      <c r="H93" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="I93" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="J93" s="69" t="s">
-        <v>65</v>
-      </c>
-      <c r="K93" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="M93" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="N93" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="O93" s="69" t="s">
-        <v>65</v>
-      </c>
-      <c r="P93" s="69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="20"/>
-      <c r="B94" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="C94" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="D94" s="8"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="27"/>
-      <c r="H94" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="I94" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J94" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K94" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="M94" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="N94" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="O94" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="P94" s="8" t="s">
+      <c r="H100" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="I100" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="K100" s="78" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" s="5" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="20"/>
-      <c r="B95" s="70" t="s">
+      <c r="L100" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="C95" s="70" t="s">
+      <c r="M100" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="D95" s="8"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="27"/>
-      <c r="H95" s="27"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="7"/>
-      <c r="K95" s="8"/>
-      <c r="M95" s="27"/>
-      <c r="N95" s="8"/>
-      <c r="O95" s="7"/>
-      <c r="P95" s="8"/>
-    </row>
-    <row r="96" spans="1:16" s="5" customFormat="1" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B96" s="8" t="str">
-        <f ca="1">INDEX(INDIRECT(B$95),
-     MATCH($B$93, INDIRECT(B$95&amp;"_Color"), 0),
-     MATCH($A96, INDIRECT(B$95&amp;"_H"), 0)
+      <c r="N100" s="77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" s="5" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="20"/>
+      <c r="B101" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="C101" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="D101" s="8"/>
+      <c r="E101" s="7"/>
+    </row>
+    <row r="102" spans="1:14" s="5" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102" s="8" t="str">
+        <f ca="1">INDEX(INDIRECT(B$101),
+     MATCH($B$99, INDIRECT(B$101&amp;"_Color"), 0),
+     MATCH($A102, INDIRECT(B$101&amp;"_H"), 0)
 )</f>
         <v>ž</v>
       </c>
-      <c r="C96" s="8" t="str">
-        <f ca="1">INDEX(INDIRECT(C$95),
-     MATCH($B$93, INDIRECT(C$95&amp;"_Color"), 0),
-     MATCH($A96, INDIRECT(C$95&amp;"_H"), 0)
+      <c r="C102" s="8" t="str">
+        <f ca="1">INDEX(INDIRECT(C$101),
+     MATCH($B$99, INDIRECT(C$101&amp;"_Color"), 0),
+     MATCH($A102, INDIRECT(C$101&amp;"_H"), 0)
 )</f>
         <v>t</v>
       </c>
-      <c r="D96" s="8"/>
-      <c r="E96" s="7"/>
-      <c r="H96" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="I96" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J96" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K96" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="M96" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="N96" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="O96" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="P96" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D97" s="8"/>
-      <c r="E97" s="7"/>
-      <c r="H97" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="I97" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J97" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K97" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="M97" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="N97" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="O97" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="P97" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C98" s="7"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="7"/>
-      <c r="H98" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="I98" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="J98" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="K98" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="M98" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="N98" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="O98" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="P98" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="40"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="7"/>
-      <c r="H99" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="I99" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J99" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="K99" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="M99" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="N99" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="O99" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="P99" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="40"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="7"/>
-      <c r="H100" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="I100" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J100" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="K100" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="M100" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="N100" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="O100" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="P100" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="40"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="7"/>
-    </row>
-    <row r="102" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="C102" s="7"/>
       <c r="D102" s="8"/>
       <c r="E102" s="7"/>
-    </row>
-    <row r="103" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="42"/>
-    </row>
-    <row r="104" spans="1:16" s="72" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="71" t="s">
+      <c r="F102" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G102" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H102" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I102" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K102" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="L102" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M102" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="N102" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="8"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G103" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H103" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I103" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K103" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="L103" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M103" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="N103" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="7"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I104" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K104" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="L104" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="M104" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="N104" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="48"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H105" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I105" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="K105" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="L105" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M105" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="N105" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="48"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H106" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I106" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K106" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="L106" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M106" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="105" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="73" t="s">
+      <c r="N106" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="73" t="s">
+    <row r="107" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="48"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="27" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="107" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="74"/>
-      <c r="B107" s="47" t="s">
+      <c r="G107" s="8" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="108" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="75"/>
-      <c r="B108" s="47" t="s">
+      <c r="H107" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I107" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="109" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="76"/>
-      <c r="B109" s="47" t="s">
+      <c r="K107" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="L107" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="110" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="77"/>
-      <c r="B110" s="47" t="s">
+      <c r="M107" s="8" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="111" spans="1:16" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="78"/>
-      <c r="B111" s="54" t="s">
+      <c r="N107" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="112" spans="1:16" s="79" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="113" s="79" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="114" s="79" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="115" s="79" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="116" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="117" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="118" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="119" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="120" s="81" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="108" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="48"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="7"/>
+    </row>
+    <row r="109" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C109" s="7"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="7"/>
+    </row>
+    <row r="110" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="49"/>
+    </row>
+    <row r="111" spans="1:14" s="81" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A111" s="80" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="82" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="82" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="83"/>
+      <c r="B114" s="54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="84"/>
+      <c r="B115" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="85"/>
+      <c r="B116" s="54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="86"/>
+      <c r="B117" s="54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="87"/>
+      <c r="B118" s="67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" s="88" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:2" s="88" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:2" s="88" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:2" s="88" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:2" s="90" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="129" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="130" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="131" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="132" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="133" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="134" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="135" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>